<commit_message>
Moving towards a working database
</commit_message>
<xml_diff>
--- a/book/DATA/phase1_document_to_pdf_crosswalk_filled.xlsx
+++ b/book/DATA/phase1_document_to_pdf_crosswalk_filled.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\aimoralcode-core\book\DATA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5292ED02-ED4B-4C45-99CA-FE99B4FC8EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2495,8 +2501,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2572,13 +2578,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2616,7 +2630,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2650,6 +2664,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2684,9 +2699,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2859,14 +2875,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.109375" customWidth="1"/>
+    <col min="3" max="3" width="50.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2892,7 +2916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2918,7 +2942,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2929,7 +2953,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2940,7 +2964,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2960,7 +2984,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2980,7 +3004,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3000,7 +3024,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3020,7 +3044,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3031,7 +3055,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3051,7 +3075,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3062,7 +3086,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3082,7 +3106,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -3093,7 +3117,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -3104,7 +3128,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3124,7 +3148,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3144,7 +3168,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -3164,7 +3188,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -3184,7 +3208,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3204,7 +3228,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -3224,7 +3248,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -3235,7 +3259,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -3255,7 +3279,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -3275,7 +3299,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3295,7 +3319,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3318,7 +3342,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -3338,7 +3362,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -3358,7 +3382,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -3369,7 +3393,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -3392,7 +3416,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -3412,7 +3436,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -3432,7 +3456,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -3452,7 +3476,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -3472,7 +3496,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -3492,7 +3516,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -3512,7 +3536,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -3532,7 +3556,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -3552,7 +3576,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -3572,7 +3596,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -3592,7 +3616,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -3612,7 +3636,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -3632,7 +3656,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -3652,7 +3676,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -3672,7 +3696,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -3692,7 +3716,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -3712,7 +3736,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -3732,7 +3756,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -3752,7 +3776,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -3772,7 +3796,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -3795,7 +3819,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -3815,7 +3839,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -3835,7 +3859,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -3855,7 +3879,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -3875,7 +3899,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -3895,7 +3919,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -3918,7 +3942,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -3938,7 +3962,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -3949,7 +3973,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -3969,7 +3993,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -3989,7 +4013,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -4009,7 +4033,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -4029,7 +4053,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -4049,7 +4073,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -4060,7 +4084,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -4080,7 +4104,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -4100,7 +4124,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -4120,7 +4144,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -4140,7 +4164,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -4160,7 +4184,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -4180,7 +4204,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -4200,7 +4224,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -4220,7 +4244,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -4231,7 +4255,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -4251,7 +4275,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -4262,7 +4286,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -4282,7 +4306,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -4302,7 +4326,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -4322,7 +4346,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -4342,7 +4366,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -4362,7 +4386,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -4382,7 +4406,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -4402,7 +4426,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -4422,7 +4446,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -4445,7 +4469,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -4465,7 +4489,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -4485,7 +4509,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -4505,7 +4529,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -4516,7 +4540,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -4536,7 +4560,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -4556,7 +4580,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -4576,7 +4600,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -4596,7 +4620,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -4616,7 +4640,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -4636,7 +4660,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -4656,7 +4680,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -4676,7 +4700,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -4696,7 +4720,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -4716,7 +4740,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -4727,7 +4751,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -4750,7 +4774,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -4773,7 +4797,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -4793,7 +4817,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -4813,7 +4837,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -4824,7 +4848,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -4847,7 +4871,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -4870,7 +4894,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -4890,7 +4914,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -4910,7 +4934,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -4930,7 +4954,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -4953,7 +4977,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -4973,7 +4997,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -4993,7 +5017,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -5013,7 +5037,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -5036,7 +5060,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -5059,7 +5083,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -5070,7 +5094,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -5093,7 +5117,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -5116,7 +5140,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -5127,7 +5151,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -5138,7 +5162,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -5158,7 +5182,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -5181,7 +5205,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -5201,7 +5225,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>129</v>
       </c>
@@ -5224,7 +5248,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>130</v>
       </c>
@@ -5247,7 +5271,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>131</v>
       </c>
@@ -5270,7 +5294,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>132</v>
       </c>
@@ -5290,7 +5314,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>133</v>
       </c>
@@ -5310,7 +5334,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>134</v>
       </c>
@@ -5333,7 +5357,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>135</v>
       </c>
@@ -5353,7 +5377,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>136</v>
       </c>
@@ -5373,7 +5397,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -5393,7 +5417,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>138</v>
       </c>
@@ -5413,7 +5437,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>139</v>
       </c>
@@ -5424,7 +5448,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>140</v>
       </c>
@@ -5447,7 +5471,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>141</v>
       </c>
@@ -5467,7 +5491,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>142</v>
       </c>
@@ -5487,7 +5511,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>143</v>
       </c>
@@ -5507,7 +5531,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>144</v>
       </c>
@@ -5530,7 +5554,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>145</v>
       </c>
@@ -5553,7 +5577,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>146</v>
       </c>
@@ -5564,7 +5588,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>147</v>
       </c>
@@ -5575,7 +5599,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>148</v>
       </c>
@@ -5595,7 +5619,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>149</v>
       </c>
@@ -5615,7 +5639,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>150</v>
       </c>
@@ -5638,7 +5662,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>151</v>
       </c>
@@ -5658,7 +5682,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>152</v>
       </c>
@@ -5678,7 +5702,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>153</v>
       </c>
@@ -5698,7 +5722,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>154</v>
       </c>
@@ -5709,7 +5733,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>155</v>
       </c>
@@ -5729,7 +5753,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>156</v>
       </c>
@@ -5749,7 +5773,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>157</v>
       </c>
@@ -5769,7 +5793,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>158</v>
       </c>
@@ -5792,7 +5816,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>159</v>
       </c>
@@ -5812,7 +5836,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>160</v>
       </c>
@@ -5832,7 +5856,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>161</v>
       </c>
@@ -5852,7 +5876,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>162</v>
       </c>
@@ -5872,7 +5896,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>163</v>
       </c>
@@ -5892,7 +5916,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>164</v>
       </c>
@@ -5912,7 +5936,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>165</v>
       </c>
@@ -5932,7 +5956,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>166</v>
       </c>
@@ -5952,7 +5976,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>167</v>
       </c>
@@ -5975,7 +5999,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>168</v>
       </c>
@@ -5998,7 +6022,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>169</v>
       </c>
@@ -6021,7 +6045,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>170</v>
       </c>
@@ -6044,7 +6068,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>171</v>
       </c>
@@ -6064,7 +6088,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>172</v>
       </c>
@@ -6084,7 +6108,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>173</v>
       </c>
@@ -6104,7 +6128,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>174</v>
       </c>
@@ -6124,7 +6148,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>175</v>
       </c>
@@ -6144,7 +6168,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>176</v>
       </c>
@@ -6164,7 +6188,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>177</v>
       </c>
@@ -6187,7 +6211,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>178</v>
       </c>
@@ -6210,7 +6234,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>179</v>
       </c>
@@ -6233,7 +6257,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>180</v>
       </c>
@@ -6253,7 +6277,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>181</v>
       </c>
@@ -6273,7 +6297,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>182</v>
       </c>
@@ -6293,7 +6317,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>183</v>
       </c>
@@ -6316,7 +6340,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>184</v>
       </c>
@@ -6339,7 +6363,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>185</v>
       </c>
@@ -6362,7 +6386,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>186</v>
       </c>
@@ -6382,7 +6406,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>187</v>
       </c>
@@ -6402,7 +6426,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>188</v>
       </c>
@@ -6422,7 +6446,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>189</v>
       </c>
@@ -6442,7 +6466,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>190</v>
       </c>
@@ -6462,7 +6486,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>191</v>
       </c>
@@ -6482,7 +6506,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>192</v>
       </c>
@@ -6502,7 +6526,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>193</v>
       </c>
@@ -6525,7 +6549,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>194</v>
       </c>
@@ -6536,7 +6560,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>195</v>
       </c>
@@ -6547,7 +6571,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>196</v>
       </c>
@@ -6558,7 +6582,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>197</v>
       </c>
@@ -6581,7 +6605,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>198</v>
       </c>
@@ -6604,7 +6628,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>199</v>
       </c>
@@ -6624,7 +6648,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>200</v>
       </c>
@@ -6644,7 +6668,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>201</v>
       </c>
@@ -6664,7 +6688,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>202</v>
       </c>
@@ -6684,7 +6708,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>203</v>
       </c>
@@ -6704,7 +6728,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>204</v>
       </c>
@@ -6724,7 +6748,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>205</v>
       </c>
@@ -6744,7 +6768,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>206</v>
       </c>
@@ -6764,7 +6788,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>207</v>
       </c>
@@ -6784,7 +6808,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>208</v>
       </c>
@@ -6807,7 +6831,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>209</v>
       </c>
@@ -6827,7 +6851,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>210</v>
       </c>
@@ -6847,7 +6871,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>211</v>
       </c>
@@ -6870,7 +6894,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>212</v>
       </c>
@@ -6893,7 +6917,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>213</v>
       </c>
@@ -6916,7 +6940,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>214</v>
       </c>
@@ -6939,7 +6963,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>215</v>
       </c>
@@ -6962,7 +6986,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>216</v>
       </c>
@@ -6982,7 +7006,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>217</v>
       </c>
@@ -7002,7 +7026,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>218</v>
       </c>
@@ -7013,7 +7037,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>219</v>
       </c>
@@ -7036,7 +7060,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>220</v>
       </c>
@@ -7059,7 +7083,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>221</v>
       </c>
@@ -7082,7 +7106,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>222</v>
       </c>
@@ -7093,7 +7117,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>223</v>
       </c>
@@ -7113,7 +7137,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>224</v>
       </c>
@@ -7133,7 +7157,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>225</v>
       </c>
@@ -7156,7 +7180,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>226</v>
       </c>
@@ -7167,7 +7191,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="221" spans="1:8">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>227</v>
       </c>
@@ -7187,7 +7211,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>228</v>
       </c>
@@ -7210,7 +7234,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>229</v>
       </c>
@@ -7233,7 +7257,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>230</v>
       </c>
@@ -7253,7 +7277,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>231</v>
       </c>
@@ -7276,7 +7300,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>232</v>
       </c>
@@ -7299,7 +7323,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>233</v>
       </c>
@@ -7322,7 +7346,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>234</v>
       </c>
@@ -7345,7 +7369,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>235</v>
       </c>
@@ -7368,7 +7392,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>236</v>
       </c>
@@ -7388,7 +7412,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>237</v>
       </c>
@@ -7399,7 +7423,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>238</v>
       </c>
@@ -7419,7 +7443,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>239</v>
       </c>
@@ -7430,7 +7454,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>240</v>
       </c>
@@ -7450,7 +7474,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>241</v>
       </c>
@@ -7473,7 +7497,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>242</v>
       </c>
@@ -7493,7 +7517,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>243</v>
       </c>
@@ -7513,7 +7537,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>244</v>
       </c>
@@ -7524,7 +7548,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>245</v>
       </c>
@@ -7544,7 +7568,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>246</v>
       </c>
@@ -7555,7 +7579,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>247</v>
       </c>
@@ -7575,7 +7599,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>248</v>
       </c>
@@ -7598,7 +7622,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>249</v>
       </c>
@@ -7618,7 +7642,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>250</v>
       </c>
@@ -7638,7 +7662,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="245" spans="1:8">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>251</v>
       </c>
@@ -7658,7 +7682,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>252</v>
       </c>
@@ -7678,7 +7702,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>253</v>
       </c>
@@ -7698,7 +7722,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>254</v>
       </c>
@@ -7721,7 +7745,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>255</v>
       </c>
@@ -7744,7 +7768,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>256</v>
       </c>
@@ -7767,7 +7791,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>257</v>
       </c>
@@ -7787,7 +7811,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>258</v>
       </c>
@@ -7807,7 +7831,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>259</v>
       </c>
@@ -7827,7 +7851,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>260</v>
       </c>
@@ -7838,7 +7862,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>261</v>
       </c>
@@ -7858,7 +7882,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>262</v>
       </c>
@@ -7881,7 +7905,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="257" spans="1:7">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>263</v>
       </c>
@@ -7892,7 +7916,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>264</v>
       </c>
@@ -7903,7 +7927,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>265</v>
       </c>
@@ -7923,7 +7947,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>266</v>
       </c>
@@ -7943,7 +7967,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>267</v>
       </c>
@@ -7963,7 +7987,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>268</v>
       </c>
@@ -7983,7 +8007,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="263" spans="1:7">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>269</v>
       </c>
@@ -7994,7 +8018,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>270</v>
       </c>
@@ -8014,7 +8038,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="265" spans="1:7">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>271</v>
       </c>
@@ -8025,7 +8049,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="266" spans="1:7">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>272</v>
       </c>
@@ -8045,7 +8069,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="267" spans="1:7">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>273</v>
       </c>
@@ -8065,7 +8089,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>274</v>
       </c>
@@ -8085,7 +8109,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>275</v>
       </c>
@@ -8105,7 +8129,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>276</v>
       </c>
@@ -8125,7 +8149,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>277</v>
       </c>
@@ -8145,7 +8169,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>278</v>
       </c>
@@ -8156,7 +8180,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>279</v>
       </c>
@@ -8176,7 +8200,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>280</v>
       </c>
@@ -8196,7 +8220,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>281</v>
       </c>
@@ -8216,7 +8240,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>282</v>
       </c>
@@ -8239,7 +8263,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>283</v>
       </c>
@@ -8262,7 +8286,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="278" spans="1:8">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>284</v>
       </c>
@@ -8282,7 +8306,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>285</v>
       </c>
@@ -8302,7 +8326,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>286</v>
       </c>
@@ -8325,7 +8349,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>287</v>
       </c>
@@ -8348,7 +8372,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>288</v>
       </c>
@@ -8359,7 +8383,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="283" spans="1:8">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>289</v>
       </c>
@@ -8379,7 +8403,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>290</v>
       </c>
@@ -8399,7 +8423,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="285" spans="1:8">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>291</v>
       </c>
@@ -8419,7 +8443,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>292</v>
       </c>
@@ -8430,7 +8454,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="287" spans="1:8">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>293</v>
       </c>
@@ -8450,7 +8474,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>294</v>
       </c>
@@ -8470,7 +8494,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="289" spans="1:4">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>295</v>
       </c>
@@ -8481,7 +8505,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="290" spans="1:4">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>296</v>
       </c>
@@ -8492,7 +8516,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="291" spans="1:4">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>297</v>
       </c>
@@ -8503,7 +8527,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="292" spans="1:4">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>298</v>
       </c>
@@ -8516,253 +8540,253 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G5" r:id="rId2"/>
-    <hyperlink ref="G6" r:id="rId3"/>
-    <hyperlink ref="G7" r:id="rId4"/>
-    <hyperlink ref="G8" r:id="rId5"/>
-    <hyperlink ref="G10" r:id="rId6"/>
-    <hyperlink ref="G12" r:id="rId7"/>
-    <hyperlink ref="G15" r:id="rId8"/>
-    <hyperlink ref="G16" r:id="rId9"/>
-    <hyperlink ref="G17" r:id="rId10"/>
-    <hyperlink ref="G18" r:id="rId11"/>
-    <hyperlink ref="G19" r:id="rId12"/>
-    <hyperlink ref="G20" r:id="rId13"/>
-    <hyperlink ref="G22" r:id="rId14"/>
-    <hyperlink ref="G23" r:id="rId15"/>
-    <hyperlink ref="G24" r:id="rId16"/>
-    <hyperlink ref="G25" r:id="rId17"/>
-    <hyperlink ref="G26" r:id="rId18"/>
-    <hyperlink ref="G27" r:id="rId19"/>
-    <hyperlink ref="G29" r:id="rId20"/>
-    <hyperlink ref="G30" r:id="rId21"/>
-    <hyperlink ref="G31" r:id="rId22"/>
-    <hyperlink ref="G32" r:id="rId23"/>
-    <hyperlink ref="G33" r:id="rId24"/>
-    <hyperlink ref="G34" r:id="rId25"/>
-    <hyperlink ref="G35" r:id="rId26"/>
-    <hyperlink ref="G36" r:id="rId27"/>
-    <hyperlink ref="G37" r:id="rId28"/>
-    <hyperlink ref="G38" r:id="rId29"/>
-    <hyperlink ref="G39" r:id="rId30"/>
-    <hyperlink ref="G40" r:id="rId31"/>
-    <hyperlink ref="G41" r:id="rId32"/>
-    <hyperlink ref="G42" r:id="rId33"/>
-    <hyperlink ref="G43" r:id="rId34"/>
-    <hyperlink ref="G44" r:id="rId35"/>
-    <hyperlink ref="G45" r:id="rId36"/>
-    <hyperlink ref="G46" r:id="rId37"/>
-    <hyperlink ref="G47" r:id="rId38"/>
-    <hyperlink ref="G48" r:id="rId39"/>
-    <hyperlink ref="G49" r:id="rId40"/>
-    <hyperlink ref="G50" r:id="rId41"/>
-    <hyperlink ref="G51" r:id="rId42"/>
-    <hyperlink ref="G52" r:id="rId43"/>
-    <hyperlink ref="G53" r:id="rId44"/>
-    <hyperlink ref="G54" r:id="rId45"/>
-    <hyperlink ref="G55" r:id="rId46"/>
-    <hyperlink ref="G56" r:id="rId47"/>
-    <hyperlink ref="G58" r:id="rId48"/>
-    <hyperlink ref="G59" r:id="rId49"/>
-    <hyperlink ref="G60" r:id="rId50"/>
-    <hyperlink ref="G61" r:id="rId51"/>
-    <hyperlink ref="G62" r:id="rId52"/>
-    <hyperlink ref="G64" r:id="rId53"/>
-    <hyperlink ref="G65" r:id="rId54"/>
-    <hyperlink ref="G66" r:id="rId55"/>
-    <hyperlink ref="G67" r:id="rId56"/>
-    <hyperlink ref="G68" r:id="rId57"/>
-    <hyperlink ref="G69" r:id="rId58"/>
-    <hyperlink ref="G70" r:id="rId59"/>
-    <hyperlink ref="G71" r:id="rId60"/>
-    <hyperlink ref="G73" r:id="rId61"/>
-    <hyperlink ref="G75" r:id="rId62"/>
-    <hyperlink ref="G76" r:id="rId63"/>
-    <hyperlink ref="G77" r:id="rId64"/>
-    <hyperlink ref="G78" r:id="rId65"/>
-    <hyperlink ref="G79" r:id="rId66"/>
-    <hyperlink ref="G80" r:id="rId67"/>
-    <hyperlink ref="G81" r:id="rId68"/>
-    <hyperlink ref="G82" r:id="rId69"/>
-    <hyperlink ref="G83" r:id="rId70"/>
-    <hyperlink ref="G84" r:id="rId71"/>
-    <hyperlink ref="G85" r:id="rId72"/>
-    <hyperlink ref="G86" r:id="rId73"/>
-    <hyperlink ref="G88" r:id="rId74"/>
-    <hyperlink ref="G89" r:id="rId75"/>
-    <hyperlink ref="G90" r:id="rId76"/>
-    <hyperlink ref="G91" r:id="rId77"/>
-    <hyperlink ref="G92" r:id="rId78"/>
-    <hyperlink ref="G93" r:id="rId79"/>
-    <hyperlink ref="G94" r:id="rId80"/>
-    <hyperlink ref="G95" r:id="rId81"/>
-    <hyperlink ref="G96" r:id="rId82"/>
-    <hyperlink ref="G97" r:id="rId83"/>
-    <hyperlink ref="G99" r:id="rId84"/>
-    <hyperlink ref="G100" r:id="rId85"/>
-    <hyperlink ref="G101" r:id="rId86"/>
-    <hyperlink ref="G102" r:id="rId87"/>
-    <hyperlink ref="G104" r:id="rId88"/>
-    <hyperlink ref="G105" r:id="rId89"/>
-    <hyperlink ref="G106" r:id="rId90"/>
-    <hyperlink ref="G107" r:id="rId91"/>
-    <hyperlink ref="G108" r:id="rId92"/>
-    <hyperlink ref="G109" r:id="rId93"/>
-    <hyperlink ref="G110" r:id="rId94"/>
-    <hyperlink ref="G111" r:id="rId95"/>
-    <hyperlink ref="G112" r:id="rId96"/>
-    <hyperlink ref="G113" r:id="rId97"/>
-    <hyperlink ref="G114" r:id="rId98"/>
-    <hyperlink ref="G116" r:id="rId99"/>
-    <hyperlink ref="G117" r:id="rId100"/>
-    <hyperlink ref="G120" r:id="rId101"/>
-    <hyperlink ref="G121" r:id="rId102"/>
-    <hyperlink ref="G122" r:id="rId103"/>
-    <hyperlink ref="G123" r:id="rId104"/>
-    <hyperlink ref="G124" r:id="rId105"/>
-    <hyperlink ref="G125" r:id="rId106"/>
-    <hyperlink ref="G126" r:id="rId107"/>
-    <hyperlink ref="G127" r:id="rId108"/>
-    <hyperlink ref="G128" r:id="rId109"/>
-    <hyperlink ref="G129" r:id="rId110"/>
-    <hyperlink ref="G130" r:id="rId111"/>
-    <hyperlink ref="G131" r:id="rId112"/>
-    <hyperlink ref="G132" r:id="rId113"/>
-    <hyperlink ref="G134" r:id="rId114"/>
-    <hyperlink ref="G135" r:id="rId115"/>
-    <hyperlink ref="G136" r:id="rId116"/>
-    <hyperlink ref="G137" r:id="rId117"/>
-    <hyperlink ref="G138" r:id="rId118"/>
-    <hyperlink ref="G139" r:id="rId119"/>
-    <hyperlink ref="G142" r:id="rId120"/>
-    <hyperlink ref="G143" r:id="rId121"/>
-    <hyperlink ref="G144" r:id="rId122"/>
-    <hyperlink ref="G145" r:id="rId123"/>
-    <hyperlink ref="G146" r:id="rId124"/>
-    <hyperlink ref="G147" r:id="rId125"/>
-    <hyperlink ref="G149" r:id="rId126"/>
-    <hyperlink ref="G150" r:id="rId127"/>
-    <hyperlink ref="G151" r:id="rId128"/>
-    <hyperlink ref="G152" r:id="rId129"/>
-    <hyperlink ref="G153" r:id="rId130"/>
-    <hyperlink ref="G154" r:id="rId131"/>
-    <hyperlink ref="G155" r:id="rId132"/>
-    <hyperlink ref="G156" r:id="rId133"/>
-    <hyperlink ref="G157" r:id="rId134"/>
-    <hyperlink ref="G158" r:id="rId135"/>
-    <hyperlink ref="G159" r:id="rId136"/>
-    <hyperlink ref="G160" r:id="rId137"/>
-    <hyperlink ref="G161" r:id="rId138"/>
-    <hyperlink ref="G162" r:id="rId139"/>
-    <hyperlink ref="G163" r:id="rId140"/>
-    <hyperlink ref="G164" r:id="rId141"/>
-    <hyperlink ref="G165" r:id="rId142"/>
-    <hyperlink ref="G166" r:id="rId143"/>
-    <hyperlink ref="G167" r:id="rId144"/>
-    <hyperlink ref="G168" r:id="rId145"/>
-    <hyperlink ref="G169" r:id="rId146"/>
-    <hyperlink ref="G170" r:id="rId147"/>
-    <hyperlink ref="G171" r:id="rId148"/>
-    <hyperlink ref="G172" r:id="rId149"/>
-    <hyperlink ref="G173" r:id="rId150"/>
-    <hyperlink ref="G174" r:id="rId151"/>
-    <hyperlink ref="G175" r:id="rId152"/>
-    <hyperlink ref="G176" r:id="rId153"/>
-    <hyperlink ref="G177" r:id="rId154"/>
-    <hyperlink ref="G178" r:id="rId155"/>
-    <hyperlink ref="G179" r:id="rId156"/>
-    <hyperlink ref="G180" r:id="rId157"/>
-    <hyperlink ref="G181" r:id="rId158"/>
-    <hyperlink ref="G182" r:id="rId159"/>
-    <hyperlink ref="G183" r:id="rId160"/>
-    <hyperlink ref="G184" r:id="rId161"/>
-    <hyperlink ref="G185" r:id="rId162"/>
-    <hyperlink ref="G186" r:id="rId163"/>
-    <hyperlink ref="G187" r:id="rId164"/>
-    <hyperlink ref="G191" r:id="rId165"/>
-    <hyperlink ref="G192" r:id="rId166"/>
-    <hyperlink ref="G193" r:id="rId167"/>
-    <hyperlink ref="G194" r:id="rId168"/>
-    <hyperlink ref="G195" r:id="rId169"/>
-    <hyperlink ref="G196" r:id="rId170"/>
-    <hyperlink ref="G197" r:id="rId171"/>
-    <hyperlink ref="G198" r:id="rId172"/>
-    <hyperlink ref="G199" r:id="rId173"/>
-    <hyperlink ref="G200" r:id="rId174"/>
-    <hyperlink ref="G201" r:id="rId175"/>
-    <hyperlink ref="G202" r:id="rId176"/>
-    <hyperlink ref="G203" r:id="rId177"/>
-    <hyperlink ref="G204" r:id="rId178"/>
-    <hyperlink ref="G205" r:id="rId179"/>
-    <hyperlink ref="G206" r:id="rId180"/>
-    <hyperlink ref="G207" r:id="rId181"/>
-    <hyperlink ref="G208" r:id="rId182"/>
-    <hyperlink ref="G209" r:id="rId183"/>
-    <hyperlink ref="G210" r:id="rId184"/>
-    <hyperlink ref="G211" r:id="rId185"/>
-    <hyperlink ref="G213" r:id="rId186"/>
-    <hyperlink ref="G214" r:id="rId187"/>
-    <hyperlink ref="G215" r:id="rId188"/>
-    <hyperlink ref="G217" r:id="rId189"/>
-    <hyperlink ref="G218" r:id="rId190"/>
-    <hyperlink ref="G219" r:id="rId191"/>
-    <hyperlink ref="G221" r:id="rId192"/>
-    <hyperlink ref="G222" r:id="rId193"/>
-    <hyperlink ref="G223" r:id="rId194"/>
-    <hyperlink ref="G224" r:id="rId195"/>
-    <hyperlink ref="G225" r:id="rId196"/>
-    <hyperlink ref="G226" r:id="rId197"/>
-    <hyperlink ref="G227" r:id="rId198"/>
-    <hyperlink ref="G228" r:id="rId199"/>
-    <hyperlink ref="G229" r:id="rId200"/>
-    <hyperlink ref="G230" r:id="rId201"/>
-    <hyperlink ref="G232" r:id="rId202"/>
-    <hyperlink ref="G234" r:id="rId203"/>
-    <hyperlink ref="G235" r:id="rId204"/>
-    <hyperlink ref="G236" r:id="rId205"/>
-    <hyperlink ref="G237" r:id="rId206"/>
-    <hyperlink ref="G239" r:id="rId207"/>
-    <hyperlink ref="G241" r:id="rId208"/>
-    <hyperlink ref="G242" r:id="rId209"/>
-    <hyperlink ref="G243" r:id="rId210"/>
-    <hyperlink ref="G244" r:id="rId211"/>
-    <hyperlink ref="G245" r:id="rId212"/>
-    <hyperlink ref="G246" r:id="rId213"/>
-    <hyperlink ref="G247" r:id="rId214"/>
-    <hyperlink ref="G248" r:id="rId215"/>
-    <hyperlink ref="G249" r:id="rId216"/>
-    <hyperlink ref="G250" r:id="rId217"/>
-    <hyperlink ref="G251" r:id="rId218"/>
-    <hyperlink ref="G252" r:id="rId219"/>
-    <hyperlink ref="G253" r:id="rId220"/>
-    <hyperlink ref="G255" r:id="rId221"/>
-    <hyperlink ref="G256" r:id="rId222"/>
-    <hyperlink ref="G259" r:id="rId223"/>
-    <hyperlink ref="G260" r:id="rId224"/>
-    <hyperlink ref="G261" r:id="rId225"/>
-    <hyperlink ref="G262" r:id="rId226"/>
-    <hyperlink ref="G264" r:id="rId227"/>
-    <hyperlink ref="G266" r:id="rId228"/>
-    <hyperlink ref="G267" r:id="rId229"/>
-    <hyperlink ref="G268" r:id="rId230"/>
-    <hyperlink ref="G269" r:id="rId231"/>
-    <hyperlink ref="G270" r:id="rId232"/>
-    <hyperlink ref="G271" r:id="rId233"/>
-    <hyperlink ref="G273" r:id="rId234"/>
-    <hyperlink ref="G274" r:id="rId235"/>
-    <hyperlink ref="G275" r:id="rId236"/>
-    <hyperlink ref="G276" r:id="rId237"/>
-    <hyperlink ref="G277" r:id="rId238"/>
-    <hyperlink ref="G278" r:id="rId239"/>
-    <hyperlink ref="G279" r:id="rId240"/>
-    <hyperlink ref="G280" r:id="rId241"/>
-    <hyperlink ref="G281" r:id="rId242"/>
-    <hyperlink ref="G283" r:id="rId243"/>
-    <hyperlink ref="G284" r:id="rId244"/>
-    <hyperlink ref="G285" r:id="rId245"/>
-    <hyperlink ref="G287" r:id="rId246"/>
-    <hyperlink ref="G288" r:id="rId247"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G30" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G31" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G32" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G33" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G34" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G35" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G36" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G37" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G38" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G39" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G40" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G41" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G42" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G43" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="G44" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="G45" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="G46" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G47" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="G48" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="G49" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="G50" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="G51" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="G52" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="G53" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="G54" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="G55" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="G56" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="G58" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="G59" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="G60" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="G61" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="G62" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="G64" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G65" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="G66" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="G67" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="G68" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="G69" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="G70" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="G71" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="G73" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="G75" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="G76" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="G77" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="G78" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="G79" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="G80" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="G81" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="G82" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="G83" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="G84" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="G85" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="G86" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="G88" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="G89" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="G90" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="G91" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="G92" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="G93" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="G94" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="G95" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="G96" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="G97" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="G99" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="G100" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="G101" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="G102" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="G104" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="G105" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="G106" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="G107" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="G108" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="G109" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="G110" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="G111" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="G112" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="G113" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="G114" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="G116" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="G117" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="G120" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="G121" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="G122" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="G123" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="G124" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="G125" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="G126" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="G127" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="G128" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="G129" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="G130" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="G131" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="G132" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="G134" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="G135" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="G136" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="G137" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="G138" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="G139" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="G142" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="G143" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="G144" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="G145" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="G146" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="G147" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="G149" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="G150" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="G151" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="G152" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="G153" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="G154" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="G155" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="G156" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="G157" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="G158" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="G159" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="G160" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="G161" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="G162" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="G163" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="G164" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="G165" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="G166" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="G167" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="G168" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="G169" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="G170" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="G171" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="G172" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="G173" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="G174" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="G175" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="G176" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="G177" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="G178" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="G179" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="G180" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="G181" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="G182" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="G183" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="G184" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="G185" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="G186" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="G187" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="G191" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="G192" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="G193" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="G194" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="G195" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="G196" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="G197" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="G198" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="G199" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="G200" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="G201" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="G202" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="G203" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="G204" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="G205" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="G206" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="G207" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="G208" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="G209" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="G210" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="G211" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="G213" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="G214" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="G215" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="G217" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="G218" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="G219" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="G221" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="G222" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="G223" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="G224" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="G225" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="G226" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="G227" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="G228" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="G229" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="G230" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="G232" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="G234" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="G235" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="G236" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="G237" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="G239" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="G241" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="G242" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="G243" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="G244" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="G245" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="G246" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="G247" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="G248" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="G249" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="G250" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="G251" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="G252" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="G253" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="G255" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="G256" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="G259" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="G260" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="G261" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="G262" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="G264" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="G266" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="G267" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="G268" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="G269" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="G270" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="G271" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="G273" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="G274" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="G275" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="G276" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="G277" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="G278" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="G279" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="G280" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="G281" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="G283" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="G284" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="G285" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="G287" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="G288" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>